<commit_message>
add wrong result tests
</commit_message>
<xml_diff>
--- a/src/test/java/com/example/telephony/data/exel/correct/correct_cell_type.xlsx
+++ b/src/test/java/com/example/telephony/data/exel/correct/correct_cell_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserFiles\MyFiles\Projects\Java\Telephony\src\test\java\com\example\telephony\data\exel\correct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9766C34-EFE4-4E06-A6D4-BE2E851E9189}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93751394-C8B5-48DE-9EAB-C8B48AC3EA68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4860" yWindow="360" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>номер телефона</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>cvds</t>
+  </si>
+  <si>
+    <t>one two three</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -376,7 +382,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,11 +400,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>123</v>
-      </c>
-      <c r="E1" s="1">
-        <v>41223</v>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>